<commit_message>
feat: update lettings materials
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-lettings-legacy-template-2023-24.xlsx
+++ b/public/files/bulk-upload-lettings-legacy-template-2023-24.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="289">
   <si>
     <t>Question</t>
   </si>
@@ -536,7 +536,7 @@
     <t>Make sure the tenant has seen the attached privacy notice before completing this log</t>
   </si>
   <si>
-    <t>This is a letting to the same tenant in the same property</t>
+    <t>A renewal is a letting to the same tenant in the same property. If the property was previously being used as temporary accommodation, then answer 'no'.</t>
   </si>
   <si>
     <t>General needs housing includes both self-contained and shared housing without support or specific adaptations. Supported housing includes direct access hostels, group homes, residential care and nursing homes.</t>
@@ -849,7 +849,7 @@
     <t>Yes, if letting is a renewal (if field 6 = 1) or a first-time let (if field 27 = 15 - 17)</t>
   </si>
   <si>
-    <t>Yes, if letting is supported housing (if field 4 = 2) or if property's UPRN and local authority are known (if fields 18 and 25 are not empty)</t>
+    <t>Yes, if letting is supported housing (if field 4 = 2) or if property's UPRN or local authority is known (if field 18 or 25 is not empty)</t>
   </si>
   <si>
     <t>Yes, if no one in the household is a current or former regular (if field 79 is not 1)</t>
@@ -871,7 +871,10 @@
     <t>Yes, if letting is general needs (if field 4 = 1) or if management code is provided (if field 15 is not empty)</t>
   </si>
   <si>
-    <t>Yes, if letting is supported housing (if field 4 = 2) or if the property's postcode is not empty (if fields 23 and 24 contain full and valid entries)</t>
+    <t>Yes, if letting is supported housing (if field 4 = 2) or if the property's address is known (if fields 19, 21, 23 and 24 contain full and valid entries)</t>
+  </si>
+  <si>
+    <t>Yes, if letting is supported housing (if field 4 = 2) or if property's UPRN is known (if field 18 is not empty)</t>
   </si>
   <si>
     <t>Type of letting the question applies to</t>
@@ -1420,6 +1423,7 @@
     <col customWidth="1" min="118" max="118" width="13.5"/>
     <col customWidth="1" min="128" max="128" width="12.88"/>
     <col customWidth="1" min="132" max="132" width="13.63"/>
+    <col customWidth="1" min="135" max="135" width="13.25"/>
     <col customWidth="1" min="136" max="136" width="16.5"/>
     <col customWidth="1" min="138" max="138" width="17.38"/>
   </cols>
@@ -2702,13 +2706,13 @@
         <v>280</v>
       </c>
       <c r="EI4" s="20" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="EJ4" s="29" t="s">
         <v>226</v>
       </c>
       <c r="EK4" s="20" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="EL4" s="20" t="s">
         <v>226</v>
@@ -2716,13 +2720,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="30" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="20"/>
@@ -2806,7 +2810,7 @@
       <c r="CG5" s="20"/>
       <c r="CH5" s="31"/>
       <c r="CI5" s="32" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CJ5" s="31"/>
       <c r="CK5" s="31"/>
@@ -2823,7 +2827,7 @@
       <c r="CV5" s="20"/>
       <c r="CW5" s="20"/>
       <c r="CX5" s="23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CY5" s="13"/>
       <c r="CZ5" s="13"/>
@@ -2831,7 +2835,7 @@
       <c r="DB5" s="14"/>
       <c r="DC5" s="20"/>
       <c r="DD5" s="23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="DE5" s="13"/>
       <c r="DF5" s="14"/>
@@ -2843,7 +2847,7 @@
       <c r="DL5" s="20"/>
       <c r="DM5" s="31"/>
       <c r="DN5" s="20" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="DO5" s="31"/>
       <c r="DP5" s="31"/>
@@ -2857,10 +2861,10 @@
       <c r="DX5" s="31"/>
       <c r="DY5" s="31"/>
       <c r="DZ5" s="20" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="EA5" s="23" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="EB5" s="14"/>
       <c r="EC5" s="24"/>
@@ -2868,10 +2872,10 @@
       <c r="EE5" s="19"/>
       <c r="EF5" s="19"/>
       <c r="EG5" s="20" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="EH5" s="23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="EI5" s="13"/>
       <c r="EJ5" s="13"/>
@@ -2880,7 +2884,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34"/>
@@ -2991,9 +2995,7 @@
       <c r="CT6" s="13"/>
       <c r="CU6" s="14"/>
       <c r="CV6" s="36"/>
-      <c r="CW6" s="32" t="s">
-        <v>226</v>
-      </c>
+      <c r="CW6" s="32"/>
       <c r="CX6" s="39"/>
       <c r="CY6" s="38"/>
       <c r="CZ6" s="39"/>
@@ -3040,7 +3042,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B7" s="42">
         <v>5.0</v>
@@ -3454,26 +3456,26 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="AU3:AV3"/>
     <mergeCell ref="BD3:BI3"/>
     <mergeCell ref="BS3:BW3"/>
     <mergeCell ref="BX3:BZ3"/>
     <mergeCell ref="CC3:CH3"/>
+    <mergeCell ref="CZ3:DA3"/>
     <mergeCell ref="DP3:DY3"/>
     <mergeCell ref="DZ3:EA3"/>
+    <mergeCell ref="EE3:EF3"/>
     <mergeCell ref="EI3:EJ3"/>
     <mergeCell ref="EK3:EL3"/>
-    <mergeCell ref="CZ3:DA3"/>
-    <mergeCell ref="EE3:EF3"/>
     <mergeCell ref="N2:T2"/>
     <mergeCell ref="AC2:AI2"/>
+    <mergeCell ref="AR2:AS2"/>
     <mergeCell ref="CL2:CN2"/>
     <mergeCell ref="CO2:CQ2"/>
     <mergeCell ref="N3:T3"/>
     <mergeCell ref="U3:AB3"/>
     <mergeCell ref="AC3:AI3"/>
-    <mergeCell ref="AR2:AS2"/>
     <mergeCell ref="AJ3:AQ3"/>
-    <mergeCell ref="AU3:AV3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="AR4:AT4"/>
     <mergeCell ref="AV4:AX4"/>
@@ -3487,18 +3489,18 @@
     <mergeCell ref="BS4:BW4"/>
     <mergeCell ref="BX4:BZ4"/>
     <mergeCell ref="CD4:CF4"/>
+    <mergeCell ref="CX5:DB5"/>
+    <mergeCell ref="DD5:DF5"/>
     <mergeCell ref="EA5:EB5"/>
     <mergeCell ref="EH5:EL5"/>
-    <mergeCell ref="EE4:EF4"/>
-    <mergeCell ref="CX5:DB5"/>
-    <mergeCell ref="CY4:DA4"/>
+    <mergeCell ref="CS6:CU6"/>
     <mergeCell ref="CL4:CN4"/>
     <mergeCell ref="CO4:CQ4"/>
     <mergeCell ref="CS4:CU4"/>
+    <mergeCell ref="CY4:DA4"/>
     <mergeCell ref="DE4:DF4"/>
     <mergeCell ref="DP4:DY4"/>
-    <mergeCell ref="DD5:DF5"/>
-    <mergeCell ref="CS6:CU6"/>
+    <mergeCell ref="EE4:EF4"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
CLDC-2774 Update lettings materials (#1939)
* feat: update lettings materials

* feat: update tests

* refactor: lint
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-lettings-legacy-template-2023-24.xlsx
+++ b/public/files/bulk-upload-lettings-legacy-template-2023-24.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="289">
   <si>
     <t>Question</t>
   </si>
@@ -536,7 +536,7 @@
     <t>Make sure the tenant has seen the attached privacy notice before completing this log</t>
   </si>
   <si>
-    <t>This is a letting to the same tenant in the same property</t>
+    <t>A renewal is a letting to the same tenant in the same property. If the property was previously being used as temporary accommodation, then answer 'no'.</t>
   </si>
   <si>
     <t>General needs housing includes both self-contained and shared housing without support or specific adaptations. Supported housing includes direct access hostels, group homes, residential care and nursing homes.</t>
@@ -849,7 +849,7 @@
     <t>Yes, if letting is a renewal (if field 6 = 1) or a first-time let (if field 27 = 15 - 17)</t>
   </si>
   <si>
-    <t>Yes, if letting is supported housing (if field 4 = 2) or if property's UPRN and local authority are known (if fields 18 and 25 are not empty)</t>
+    <t>Yes, if letting is supported housing (if field 4 = 2) or if property's UPRN or local authority is known (if field 18 or 25 is not empty)</t>
   </si>
   <si>
     <t>Yes, if no one in the household is a current or former regular (if field 79 is not 1)</t>
@@ -871,7 +871,10 @@
     <t>Yes, if letting is general needs (if field 4 = 1) or if management code is provided (if field 15 is not empty)</t>
   </si>
   <si>
-    <t>Yes, if letting is supported housing (if field 4 = 2) or if the property's postcode is not empty (if fields 23 and 24 contain full and valid entries)</t>
+    <t>Yes, if letting is supported housing (if field 4 = 2) or if the property's address is known (if fields 19, 21, 23 and 24 contain full and valid entries)</t>
+  </si>
+  <si>
+    <t>Yes, if letting is supported housing (if field 4 = 2) or if property's UPRN is known (if field 18 is not empty)</t>
   </si>
   <si>
     <t>Type of letting the question applies to</t>
@@ -1420,6 +1423,7 @@
     <col customWidth="1" min="118" max="118" width="13.5"/>
     <col customWidth="1" min="128" max="128" width="12.88"/>
     <col customWidth="1" min="132" max="132" width="13.63"/>
+    <col customWidth="1" min="135" max="135" width="13.25"/>
     <col customWidth="1" min="136" max="136" width="16.5"/>
     <col customWidth="1" min="138" max="138" width="17.38"/>
   </cols>
@@ -2702,13 +2706,13 @@
         <v>280</v>
       </c>
       <c r="EI4" s="20" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="EJ4" s="29" t="s">
         <v>226</v>
       </c>
       <c r="EK4" s="20" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="EL4" s="20" t="s">
         <v>226</v>
@@ -2716,13 +2720,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="30" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="20"/>
@@ -2806,7 +2810,7 @@
       <c r="CG5" s="20"/>
       <c r="CH5" s="31"/>
       <c r="CI5" s="32" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CJ5" s="31"/>
       <c r="CK5" s="31"/>
@@ -2823,7 +2827,7 @@
       <c r="CV5" s="20"/>
       <c r="CW5" s="20"/>
       <c r="CX5" s="23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CY5" s="13"/>
       <c r="CZ5" s="13"/>
@@ -2831,7 +2835,7 @@
       <c r="DB5" s="14"/>
       <c r="DC5" s="20"/>
       <c r="DD5" s="23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="DE5" s="13"/>
       <c r="DF5" s="14"/>
@@ -2843,7 +2847,7 @@
       <c r="DL5" s="20"/>
       <c r="DM5" s="31"/>
       <c r="DN5" s="20" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="DO5" s="31"/>
       <c r="DP5" s="31"/>
@@ -2857,10 +2861,10 @@
       <c r="DX5" s="31"/>
       <c r="DY5" s="31"/>
       <c r="DZ5" s="20" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="EA5" s="23" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="EB5" s="14"/>
       <c r="EC5" s="24"/>
@@ -2868,10 +2872,10 @@
       <c r="EE5" s="19"/>
       <c r="EF5" s="19"/>
       <c r="EG5" s="20" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="EH5" s="23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="EI5" s="13"/>
       <c r="EJ5" s="13"/>
@@ -2880,7 +2884,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34"/>
@@ -2991,9 +2995,7 @@
       <c r="CT6" s="13"/>
       <c r="CU6" s="14"/>
       <c r="CV6" s="36"/>
-      <c r="CW6" s="32" t="s">
-        <v>226</v>
-      </c>
+      <c r="CW6" s="32"/>
       <c r="CX6" s="39"/>
       <c r="CY6" s="38"/>
       <c r="CZ6" s="39"/>
@@ -3040,7 +3042,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B7" s="42">
         <v>5.0</v>
@@ -3454,26 +3456,26 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="AU3:AV3"/>
     <mergeCell ref="BD3:BI3"/>
     <mergeCell ref="BS3:BW3"/>
     <mergeCell ref="BX3:BZ3"/>
     <mergeCell ref="CC3:CH3"/>
+    <mergeCell ref="CZ3:DA3"/>
     <mergeCell ref="DP3:DY3"/>
     <mergeCell ref="DZ3:EA3"/>
+    <mergeCell ref="EE3:EF3"/>
     <mergeCell ref="EI3:EJ3"/>
     <mergeCell ref="EK3:EL3"/>
-    <mergeCell ref="CZ3:DA3"/>
-    <mergeCell ref="EE3:EF3"/>
     <mergeCell ref="N2:T2"/>
     <mergeCell ref="AC2:AI2"/>
+    <mergeCell ref="AR2:AS2"/>
     <mergeCell ref="CL2:CN2"/>
     <mergeCell ref="CO2:CQ2"/>
     <mergeCell ref="N3:T3"/>
     <mergeCell ref="U3:AB3"/>
     <mergeCell ref="AC3:AI3"/>
-    <mergeCell ref="AR2:AS2"/>
     <mergeCell ref="AJ3:AQ3"/>
-    <mergeCell ref="AU3:AV3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="AR4:AT4"/>
     <mergeCell ref="AV4:AX4"/>
@@ -3487,18 +3489,18 @@
     <mergeCell ref="BS4:BW4"/>
     <mergeCell ref="BX4:BZ4"/>
     <mergeCell ref="CD4:CF4"/>
+    <mergeCell ref="CX5:DB5"/>
+    <mergeCell ref="DD5:DF5"/>
     <mergeCell ref="EA5:EB5"/>
     <mergeCell ref="EH5:EL5"/>
-    <mergeCell ref="EE4:EF4"/>
-    <mergeCell ref="CX5:DB5"/>
-    <mergeCell ref="CY4:DA4"/>
+    <mergeCell ref="CS6:CU6"/>
     <mergeCell ref="CL4:CN4"/>
     <mergeCell ref="CO4:CQ4"/>
     <mergeCell ref="CS4:CU4"/>
+    <mergeCell ref="CY4:DA4"/>
     <mergeCell ref="DE4:DF4"/>
     <mergeCell ref="DP4:DY4"/>
-    <mergeCell ref="DD5:DF5"/>
-    <mergeCell ref="CS6:CU6"/>
+    <mergeCell ref="EE4:EF4"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>